<commit_message>
Proceso de vista: view:html
</commit_message>
<xml_diff>
--- a/Documentación/Seguimiento Proyecto.xlsx
+++ b/Documentación/Seguimiento Proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Downloads\Comparador-Bicicletas\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3062F2-D632-4CBD-A709-30E005073809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13CF5C7-05CC-4333-A4E2-A8C9C614C3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="1356" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -683,7 +683,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -747,7 +747,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>

</xml_diff>

<commit_message>
Excel con información y página view.html
Excel informativo con las horas empleadas y el progreso de lo que llevo
</commit_message>
<xml_diff>
--- a/Documentación/Seguimiento Proyecto.xlsx
+++ b/Documentación/Seguimiento Proyecto.xlsx
@@ -1,26 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Downloads\Comparador-Bicicletas\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13CF5C7-05CC-4333-A4E2-A8C9C614C3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D84BE2A-3334-4927-9FF9-12A9B82D6AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1356" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tareas Proyecto" sheetId="1" r:id="rId1"/>
+    <sheet name="Control de tiempo total " sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>Tarea</t>
   </si>
@@ -31,12 +45,6 @@
     <t>Estado</t>
   </si>
   <si>
-    <t>Fecha de Inicio</t>
-  </si>
-  <si>
-    <t>Fecha de Fin</t>
-  </si>
-  <si>
     <t>Definir requisitos</t>
   </si>
   <si>
@@ -116,6 +124,51 @@
   </si>
   <si>
     <t>Crear la interfaz con Thymeleaf y Tailwind CSS</t>
+  </si>
+  <si>
+    <t>Descripción de lo realizado</t>
+  </si>
+  <si>
+    <t>Tiempo Implementado</t>
+  </si>
+  <si>
+    <t>Estructura del proyecto,Entidades y demás</t>
+  </si>
+  <si>
+    <t>Preparación del proyecto</t>
+  </si>
+  <si>
+    <t>Tiempo Total(mins)</t>
+  </si>
+  <si>
+    <t>Tiempo Total(horas)</t>
+  </si>
+  <si>
+    <t>Creación de las entidades, relaciones y ENUMS</t>
+  </si>
+  <si>
+    <t>Creación de los beans repository,service, controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creación de la pantalla principal(index.html) </t>
+  </si>
+  <si>
+    <t>Ver algunas funciones básicas de estilo Tailwind CSS</t>
+  </si>
+  <si>
+    <t>Información de ejemplo para ver como queda</t>
+  </si>
+  <si>
+    <t>Logo de la aplicación</t>
+  </si>
+  <si>
+    <t>Vista específica de una bici(view.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realizar este excel </t>
+  </si>
+  <si>
+    <t>Realizar un readme con lo que va a ser el proyecto</t>
   </si>
 </sst>
 </file>
@@ -139,15 +192,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -168,11 +227,96 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -183,11 +327,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="17">
     <dxf>
       <fill>
         <patternFill>
@@ -210,42 +381,98 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -380,14 +607,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A024E3EF-26FF-43A1-83D1-69643BA8A118}" name="Tabla1" displayName="Tabla1" ref="A1:E13" insertRowShift="1" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
-  <autoFilter ref="A1:E13" xr:uid="{A024E3EF-26FF-43A1-83D1-69643BA8A118}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A5DBCF8F-4BC1-4879-B689-2D77A586A005}" name="Tarea" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{458DB65B-2E4E-443C-8FEC-7BC129152EF6}" name="Descripción" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{49B8059D-F37C-43FB-815B-796F5E666653}" name="Estado" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{204DDDF5-88FC-4A0B-B51B-ED99259AEC09}" name="Fecha de Inicio" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{197B94E6-225F-4E56-9E6A-F85B210DB0E9}" name="Fecha de Fin" dataDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A024E3EF-26FF-43A1-83D1-69643BA8A118}" name="Tabla1" displayName="Tabla1" ref="A1:C13" insertRowShift="1" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
+  <autoFilter ref="A1:C13" xr:uid="{A024E3EF-26FF-43A1-83D1-69643BA8A118}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{A5DBCF8F-4BC1-4879-B689-2D77A586A005}" name="Tarea" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{458DB65B-2E4E-443C-8FEC-7BC129152EF6}" name="Descripción" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{49B8059D-F37C-43FB-815B-796F5E666653}" name="Estado" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{19962928-C5C1-43B1-92B1-2C63E0C2A118}" name="Tabla2" displayName="Tabla2" ref="A1:B12" totalsRowShown="0" headerRowDxfId="3" dataDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:B12" xr:uid="{19962928-C5C1-43B1-92B1-2C63E0C2A118}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{1DDBE78C-C9B3-40FF-B03A-2C1D9BBAC48D}" name="Descripción de lo realizado" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{604AB29D-9991-48B3-9503-96998609FA2F}" name="Tiempo Implementado" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -680,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -691,12 +927,10 @@
     <col min="1" max="1" width="28.54296875" style="1" customWidth="1"/>
     <col min="2" max="2" width="46.08984375" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.6328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.08984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.6328125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="4" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -706,168 +940,138 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="C11" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="C12" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
@@ -887,4 +1091,148 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D838C3E-A55D-4EF8-9723-98E491DBCC69}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="179" style="4" customWidth="1"/>
+    <col min="2" max="2" width="34.6328125" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="10.90625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="10">
+        <v>15</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="10">
+        <v>180</v>
+      </c>
+      <c r="E5" s="6">
+        <f>SUM(B2:B1048576)</f>
+        <v>1000</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6">
+        <f>E5/60</f>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="10">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="10">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="10">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>